<commit_message>
Working test of DB and PR interfaces. Still needs to be filled out.
</commit_message>
<xml_diff>
--- a/java/RoperALZIntake/RoperSpreadSheet.xlsx
+++ b/java/RoperALZIntake/RoperSpreadSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\git\rsfh-alz-intake-b\java\RoperALZIntake\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF7C5B10-6B67-4889-9D4E-E5F26F919165}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E433A6-3657-4B3D-80E3-805958AF3055}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,8 +18,8 @@
     <sheet name="OptInEamils" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_newdatabase.xlsxTable1" hidden="1">Table1[]</definedName>
-    <definedName name="_xlcn.WorksheetConnection_newdatabase.xlsxTable2" hidden="1">Table2[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_newdatabase.xlsxTable11" hidden="1">Table1[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_newdatabase.xlsxTable21" hidden="1">Table2[]</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -56,7 +56,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Table1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_newdatabase.xlsxTable1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_newdatabase.xlsxTable11"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -65,7 +65,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Table2">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_newdatabase.xlsxTable2"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_newdatabase.xlsxTable21"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="50">
   <si>
     <t>Last Name</t>
   </si>
@@ -203,6 +203,27 @@
   </si>
   <si>
     <t>age calculator</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Franks</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Aliens</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -608,17 +629,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:U32"/>
+  <dimension ref="B3:U34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="1"/>
+    <col min="4" max="4" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" style="4" customWidth="1"/>
     <col min="7" max="7" width="9.88671875" customWidth="1"/>
     <col min="8" max="8" width="21.109375" customWidth="1"/>
@@ -673,6 +694,21 @@
       </c>
     </row>
     <row r="4" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="1">
+        <v>31933</v>
+      </c>
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" t="s">
+        <v>45</v>
+      </c>
       <c r="R4" t="s">
         <v>41</v>
       </c>
@@ -822,6 +858,40 @@
     <row r="32" spans="18:18" x14ac:dyDescent="0.3">
       <c r="R32" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33" s="1">
+        <v>25568.791666666668</v>
+      </c>
+      <c r="F33" t="s">
+        <v>48</v>
+      </c>
+      <c r="G33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D34" s="1">
+        <v>25568.791666666668</v>
+      </c>
+      <c r="F34" t="s">
+        <v>48</v>
+      </c>
+      <c r="G34" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>